<commit_message>
Update TechLab Voorraad 4-3-2019.xlsx
Toegevoegd wat voor kolommen we nog moet maken in de DB en rekenening moet houden tijdens opbouwen van interacties met db.
</commit_message>
<xml_diff>
--- a/TechLab Voorraad 4-3-2019.xlsx
+++ b/TechLab Voorraad 4-3-2019.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bramg\Hogeschool Rotterdam\Ricardo Stam - Techlab algemeen gedeeld\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guanh\Google Drive\HR-Informatica\Github\TC1819_Verslengsnoer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="14_{C6D3A682-2FC4-4B31-8AA3-6AD24AC60D0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0DB8ADCF-3889-498F-88DB-CEC573BD1B04}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12165" xr2:uid="{50699BE7-1C76-8A41-B406-D92EB6F4EA30}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12165"/>
   </bookViews>
   <sheets>
-    <sheet name="Electronics" sheetId="7" r:id="rId1"/>
-    <sheet name="Books" sheetId="6" r:id="rId2"/>
+    <sheet name="Users" sheetId="9" r:id="rId1"/>
+    <sheet name="Borrow" sheetId="8" r:id="rId2"/>
+    <sheet name="Electronics" sheetId="7" r:id="rId3"/>
+    <sheet name="Books" sheetId="6" r:id="rId4"/>
+    <sheet name="Statestieken" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="190">
   <si>
     <t>ProductId</t>
   </si>
@@ -550,12 +552,75 @@
   </si>
   <si>
     <t>vr-coma-vrpc</t>
+  </si>
+  <si>
+    <t>_ID</t>
+  </si>
+  <si>
+    <t>FIRSTNAME</t>
+  </si>
+  <si>
+    <t>SURNAME</t>
+  </si>
+  <si>
+    <t>SCHOOL_EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>USER_TYPE</t>
+  </si>
+  <si>
+    <t>BLOCKED</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>beheer</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>CLASSCODE</t>
+  </si>
+  <si>
+    <t>P_USER_ID</t>
+  </si>
+  <si>
+    <t>P_PRODUCT_ID</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -645,7 +710,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{2C2BF05F-A2A0-41CB-BBE4-47A93B9F7EC3}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -957,11 +1022,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1250A6F4-1AFC-4B44-962C-3AA96429A94B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1681,8 +1875,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3B2470-90ED-40DB-B7FA-A06D85C28116}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2008,4 +2202,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>